<commit_message>
Results section of thesis
</commit_message>
<xml_diff>
--- a/Analysis/Data/2018 Tiles Allison's Computer.xlsx
+++ b/Analysis/Data/2018 Tiles Allison's Computer.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Tiles" sheetId="2" r:id="rId1"/>
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6388" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6401" uniqueCount="154">
   <si>
     <t>Stream</t>
   </si>
@@ -710,6 +710,30 @@
   <si>
     <t>Year</t>
   </si>
+  <si>
+    <t>Mean 2017</t>
+  </si>
+  <si>
+    <t>Mean 2018</t>
+  </si>
+  <si>
+    <t>Mean BACI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean N = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean Y = </t>
+  </si>
+  <si>
+    <t>Pre</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
 </sst>
 </file>
 
@@ -719,7 +743,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -806,20 +830,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -892,20 +909,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor theme="9" tint="0.39997558519241921"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor theme="9" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1038,22 +1043,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="9" tint="0.79998168889431442"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1145,20 +1139,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -16860,7 +16843,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" activeCellId="2" sqref="A1:C1048576 E1:E1048576 I1:I1048576"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37159,7 +37142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N677"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -73521,10 +73504,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T88"/>
+  <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="I96" sqref="I96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -73560,7 +73543,7 @@
       <c r="M1" t="s">
         <v>113</v>
       </c>
-      <c r="N1" s="78" t="s">
+      <c r="N1" s="73" t="s">
         <v>114</v>
       </c>
       <c r="O1" s="69"/>
@@ -73608,11 +73591,11 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <f xml:space="preserve"> E42 - E52</f>
+        <f t="shared" ref="M2:M11" si="0" xml:space="preserve"> E42 - E52</f>
         <v>2</v>
       </c>
       <c r="N2">
-        <f xml:space="preserve"> F42 - F52</f>
+        <f t="shared" ref="N2:N11" si="1" xml:space="preserve"> F42 - F52</f>
         <v>0</v>
       </c>
       <c r="O2" s="66"/>
@@ -73662,11 +73645,11 @@
         <v>10</v>
       </c>
       <c r="M3">
-        <f xml:space="preserve"> E43 - E53</f>
+        <f t="shared" si="0"/>
         <v>-3</v>
       </c>
       <c r="N3">
-        <f xml:space="preserve"> F43 - F53</f>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="O3" s="68"/>
@@ -73677,11 +73660,11 @@
         <v>10</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:T3" si="0" xml:space="preserve"> M3- M23</f>
+        <f t="shared" ref="S3:T3" si="2" xml:space="preserve"> M3- M23</f>
         <v>-5</v>
       </c>
       <c r="T3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-2</v>
       </c>
     </row>
@@ -73716,11 +73699,11 @@
         <v>20</v>
       </c>
       <c r="M4">
-        <f xml:space="preserve"> E44 - E54</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="N4">
-        <f xml:space="preserve"> F44 - F54</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="O4" s="68"/>
@@ -73731,11 +73714,11 @@
         <v>20</v>
       </c>
       <c r="S4">
-        <f t="shared" ref="S4:T4" si="1" xml:space="preserve"> M4- M24</f>
+        <f t="shared" ref="S4:T4" si="3" xml:space="preserve"> M4- M24</f>
         <v>15</v>
       </c>
       <c r="T4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
     </row>
@@ -73770,11 +73753,11 @@
         <v>30</v>
       </c>
       <c r="M5">
-        <f xml:space="preserve"> E45 - E55</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="N5">
-        <f xml:space="preserve"> F45 - F55</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O5" s="68"/>
@@ -73785,11 +73768,11 @@
         <v>30</v>
       </c>
       <c r="S5">
-        <f t="shared" ref="S5:T5" si="2" xml:space="preserve"> M5- M25</f>
+        <f t="shared" ref="S5:T5" si="4" xml:space="preserve"> M5- M25</f>
         <v>2</v>
       </c>
       <c r="T5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -73824,11 +73807,11 @@
         <v>40</v>
       </c>
       <c r="M6">
-        <f xml:space="preserve"> E46 - E56</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="N6">
-        <f xml:space="preserve"> F46 - F56</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O6" s="68"/>
@@ -73839,11 +73822,11 @@
         <v>40</v>
       </c>
       <c r="S6">
-        <f t="shared" ref="S6:T6" si="3" xml:space="preserve"> M6- M26</f>
+        <f t="shared" ref="S6:T6" si="5" xml:space="preserve"> M6- M26</f>
         <v>1</v>
       </c>
       <c r="T6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -73878,11 +73861,11 @@
         <v>50</v>
       </c>
       <c r="M7">
-        <f xml:space="preserve"> E47 - E57</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="N7">
-        <f xml:space="preserve"> F47 - F57</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="O7" s="68"/>
@@ -73893,11 +73876,11 @@
         <v>50</v>
       </c>
       <c r="S7">
-        <f t="shared" ref="S7:T7" si="4" xml:space="preserve"> M7- M27</f>
+        <f t="shared" ref="S7:T7" si="6" xml:space="preserve"> M7- M27</f>
         <v>0</v>
       </c>
       <c r="T7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
     </row>
@@ -73932,11 +73915,11 @@
         <v>60</v>
       </c>
       <c r="M8">
-        <f xml:space="preserve"> E48 - E58</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N8">
-        <f xml:space="preserve"> F48 - F58</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="O8" s="68"/>
@@ -73947,11 +73930,11 @@
         <v>60</v>
       </c>
       <c r="S8">
-        <f t="shared" ref="S8:T8" si="5" xml:space="preserve"> M8- M28</f>
+        <f t="shared" ref="S8:T8" si="7" xml:space="preserve"> M8- M28</f>
         <v>2</v>
       </c>
       <c r="T8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>31</v>
       </c>
     </row>
@@ -73986,11 +73969,11 @@
         <v>70</v>
       </c>
       <c r="M9">
-        <f xml:space="preserve"> E49 - E59</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="N9">
-        <f xml:space="preserve"> F49 - F59</f>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="O9" s="68"/>
@@ -74001,11 +73984,11 @@
         <v>70</v>
       </c>
       <c r="S9">
-        <f t="shared" ref="S9:T9" si="6" xml:space="preserve"> M9- M29</f>
+        <f t="shared" ref="S9:T9" si="8" xml:space="preserve"> M9- M29</f>
         <v>1</v>
       </c>
       <c r="T9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>39</v>
       </c>
     </row>
@@ -74040,11 +74023,11 @@
         <v>80</v>
       </c>
       <c r="M10">
-        <f xml:space="preserve"> E50 - E60</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N10">
-        <f xml:space="preserve"> F50 - F60</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O10" s="68"/>
@@ -74055,11 +74038,11 @@
         <v>80</v>
       </c>
       <c r="S10">
-        <f t="shared" ref="S10:T10" si="7" xml:space="preserve"> M10- M30</f>
+        <f t="shared" ref="S10:T10" si="9" xml:space="preserve"> M10- M30</f>
         <v>3</v>
       </c>
       <c r="T10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -74094,11 +74077,11 @@
         <v>90</v>
       </c>
       <c r="M11">
-        <f xml:space="preserve"> E51 - E61</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="N11">
-        <f xml:space="preserve"> F51 - F61</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="O11" s="68"/>
@@ -74109,11 +74092,11 @@
         <v>90</v>
       </c>
       <c r="S11">
-        <f t="shared" ref="S11:T11" si="8" xml:space="preserve"> M11- M31</f>
+        <f t="shared" ref="S11:T11" si="10" xml:space="preserve"> M11- M31</f>
         <v>3</v>
       </c>
       <c r="T11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
     </row>
@@ -74148,11 +74131,11 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <f xml:space="preserve"> E62 - E72</f>
+        <f t="shared" ref="M12:M21" si="11" xml:space="preserve"> E62 - E72</f>
         <v>9</v>
       </c>
       <c r="N12">
-        <f xml:space="preserve"> F62 - F72</f>
+        <f t="shared" ref="N12:N21" si="12" xml:space="preserve"> F62 - F72</f>
         <v>0</v>
       </c>
       <c r="O12" s="68"/>
@@ -74202,11 +74185,11 @@
         <v>10</v>
       </c>
       <c r="M13">
-        <f xml:space="preserve"> E63 - E73</f>
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
       <c r="N13">
-        <f xml:space="preserve"> F63 - F73</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O13" s="66"/>
@@ -74217,11 +74200,11 @@
         <v>10</v>
       </c>
       <c r="S13">
-        <f t="shared" ref="S13:T13" si="9" xml:space="preserve"> M13 - M33</f>
+        <f t="shared" ref="S13:T13" si="13" xml:space="preserve"> M13 - M33</f>
         <v>14</v>
       </c>
       <c r="T13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -74256,11 +74239,11 @@
         <v>20</v>
       </c>
       <c r="M14">
-        <f xml:space="preserve"> E64 - E74</f>
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
       <c r="N14">
-        <f xml:space="preserve"> F64 - F74</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="O14" s="68"/>
@@ -74271,11 +74254,11 @@
         <v>20</v>
       </c>
       <c r="S14">
-        <f t="shared" ref="S14:T14" si="10" xml:space="preserve"> M14 - M34</f>
+        <f t="shared" ref="S14:T14" si="14" xml:space="preserve"> M14 - M34</f>
         <v>13</v>
       </c>
       <c r="T14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
     </row>
@@ -74310,11 +74293,11 @@
         <v>30</v>
       </c>
       <c r="M15">
-        <f xml:space="preserve"> E65 - E75</f>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="N15">
-        <f xml:space="preserve"> F65 - F75</f>
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
       <c r="O15" s="68"/>
@@ -74325,11 +74308,11 @@
         <v>30</v>
       </c>
       <c r="S15">
-        <f t="shared" ref="S15:T15" si="11" xml:space="preserve"> M15 - M35</f>
+        <f t="shared" ref="S15:T15" si="15" xml:space="preserve"> M15 - M35</f>
         <v>4</v>
       </c>
       <c r="T15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>12</v>
       </c>
     </row>
@@ -74364,11 +74347,11 @@
         <v>40</v>
       </c>
       <c r="M16">
-        <f xml:space="preserve"> E66 - E76</f>
+        <f t="shared" si="11"/>
         <v>-3</v>
       </c>
       <c r="N16">
-        <f xml:space="preserve"> F66 - F76</f>
+        <f t="shared" si="12"/>
         <v>-2</v>
       </c>
       <c r="O16" s="68"/>
@@ -74379,11 +74362,11 @@
         <v>40</v>
       </c>
       <c r="S16">
-        <f t="shared" ref="S16:T16" si="12" xml:space="preserve"> M16 - M36</f>
+        <f t="shared" ref="S16:T16" si="16" xml:space="preserve"> M16 - M36</f>
         <v>-3</v>
       </c>
       <c r="T16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-2</v>
       </c>
     </row>
@@ -74418,11 +74401,11 @@
         <v>50</v>
       </c>
       <c r="M17">
-        <f xml:space="preserve"> E67 - E77</f>
+        <f t="shared" si="11"/>
         <v>-2</v>
       </c>
       <c r="N17">
-        <f xml:space="preserve"> F67 - F77</f>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="O17" s="68"/>
@@ -74433,11 +74416,11 @@
         <v>50</v>
       </c>
       <c r="S17">
-        <f t="shared" ref="S17:T17" si="13" xml:space="preserve"> M17 - M37</f>
+        <f t="shared" ref="S17:T17" si="17" xml:space="preserve"> M17 - M37</f>
         <v>-2</v>
       </c>
       <c r="T17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>6</v>
       </c>
     </row>
@@ -74472,11 +74455,11 @@
         <v>60</v>
       </c>
       <c r="M18">
-        <f xml:space="preserve"> E68 - E78</f>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="N18">
-        <f xml:space="preserve"> F68 - F78</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O18" s="68"/>
@@ -74487,11 +74470,11 @@
         <v>60</v>
       </c>
       <c r="S18">
-        <f t="shared" ref="S18:T18" si="14" xml:space="preserve"> M18 - M38</f>
+        <f t="shared" ref="S18:T18" si="18" xml:space="preserve"> M18 - M38</f>
         <v>4</v>
       </c>
       <c r="T18">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -74526,11 +74509,11 @@
         <v>70</v>
       </c>
       <c r="M19">
-        <f xml:space="preserve"> E69 - E79</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N19">
-        <f xml:space="preserve"> F69 - F79</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O19" s="68"/>
@@ -74541,11 +74524,11 @@
         <v>70</v>
       </c>
       <c r="S19">
-        <f t="shared" ref="S19:T19" si="15" xml:space="preserve"> M19 - M39</f>
+        <f t="shared" ref="S19:T19" si="19" xml:space="preserve"> M19 - M39</f>
         <v>0</v>
       </c>
       <c r="T19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -74580,11 +74563,11 @@
         <v>80</v>
       </c>
       <c r="M20">
-        <f xml:space="preserve"> E70 - E80</f>
+        <f t="shared" si="11"/>
         <v>-6</v>
       </c>
       <c r="N20">
-        <f xml:space="preserve"> F70 - F80</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O20" s="68"/>
@@ -74595,11 +74578,11 @@
         <v>80</v>
       </c>
       <c r="S20">
-        <f t="shared" ref="S20:T20" si="16" xml:space="preserve"> M20 - M40</f>
+        <f t="shared" ref="S20:T20" si="20" xml:space="preserve"> M20 - M40</f>
         <v>-7</v>
       </c>
       <c r="T20">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -74634,11 +74617,11 @@
         <v>90</v>
       </c>
       <c r="M21">
-        <f xml:space="preserve"> E71 - E81</f>
+        <f t="shared" si="11"/>
         <v>-6</v>
       </c>
       <c r="N21">
-        <f xml:space="preserve"> F71 - F81</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O21" s="68"/>
@@ -74649,11 +74632,11 @@
         <v>90</v>
       </c>
       <c r="S21">
-        <f t="shared" ref="S21:T21" si="17" xml:space="preserve"> M21 - M41</f>
+        <f t="shared" ref="S21:T21" si="21" xml:space="preserve"> M21 - M41</f>
         <v>-6</v>
       </c>
       <c r="T21">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -74768,11 +74751,11 @@
         <v>20</v>
       </c>
       <c r="M24">
-        <f t="shared" ref="M24:N24" si="18" xml:space="preserve"> E4 - E14</f>
+        <f t="shared" ref="M24:N24" si="22" xml:space="preserve"> E4 - E14</f>
         <v>2</v>
       </c>
       <c r="N24">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="O24" s="69"/>
@@ -74808,11 +74791,11 @@
         <v>30</v>
       </c>
       <c r="M25">
-        <f t="shared" ref="M25:N25" si="19" xml:space="preserve"> E5 - E15</f>
+        <f t="shared" ref="M25:N25" si="23" xml:space="preserve"> E5 - E15</f>
         <v>0</v>
       </c>
       <c r="N25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="O25" s="66"/>
@@ -74848,11 +74831,11 @@
         <v>40</v>
       </c>
       <c r="M26">
-        <f t="shared" ref="M26:N26" si="20" xml:space="preserve"> E6 - E16</f>
+        <f t="shared" ref="M26:N26" si="24" xml:space="preserve"> E6 - E16</f>
         <v>2</v>
       </c>
       <c r="N26">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="O26" s="68"/>
@@ -74888,11 +74871,11 @@
         <v>50</v>
       </c>
       <c r="M27">
-        <f t="shared" ref="M27:N27" si="21" xml:space="preserve"> E7 - E17</f>
+        <f t="shared" ref="M27:N27" si="25" xml:space="preserve"> E7 - E17</f>
         <v>-1</v>
       </c>
       <c r="N27">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="O27" s="68"/>
@@ -74928,11 +74911,11 @@
         <v>60</v>
       </c>
       <c r="M28">
-        <f t="shared" ref="M28:N28" si="22" xml:space="preserve"> E8 - E18</f>
+        <f t="shared" ref="M28:N28" si="26" xml:space="preserve"> E8 - E18</f>
         <v>-1</v>
       </c>
       <c r="N28">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O28" s="68"/>
@@ -74968,11 +74951,11 @@
         <v>70</v>
       </c>
       <c r="M29">
-        <f t="shared" ref="M29:N29" si="23" xml:space="preserve"> E9 - E19</f>
+        <f t="shared" ref="M29:N29" si="27" xml:space="preserve"> E9 - E19</f>
         <v>-2</v>
       </c>
       <c r="N29">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="O29" s="68"/>
@@ -75008,11 +74991,11 @@
         <v>80</v>
       </c>
       <c r="M30">
-        <f t="shared" ref="M30:N30" si="24" xml:space="preserve"> E10 - E20</f>
+        <f t="shared" ref="M30:N30" si="28" xml:space="preserve"> E10 - E20</f>
         <v>-2</v>
       </c>
       <c r="N30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="O30" s="68"/>
@@ -75048,11 +75031,11 @@
         <v>90</v>
       </c>
       <c r="M31">
-        <f t="shared" ref="M31:N31" si="25" xml:space="preserve"> E11 - E21</f>
+        <f t="shared" ref="M31:N31" si="29" xml:space="preserve"> E11 - E21</f>
         <v>-1</v>
       </c>
       <c r="N31">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="O31" s="68"/>
@@ -75097,7 +75080,7 @@
       </c>
       <c r="O32" s="68"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -75128,16 +75111,16 @@
         <v>10</v>
       </c>
       <c r="M33">
-        <f t="shared" ref="M33:N33" si="26" xml:space="preserve"> E23 - E33</f>
+        <f t="shared" ref="M33:N33" si="30" xml:space="preserve"> E23 - E33</f>
         <v>2</v>
       </c>
       <c r="N33">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="O33" s="68"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -75168,16 +75151,16 @@
         <v>20</v>
       </c>
       <c r="M34">
-        <f t="shared" ref="M34:N34" si="27" xml:space="preserve"> E24 - E34</f>
+        <f t="shared" ref="M34:N34" si="31" xml:space="preserve"> E24 - E34</f>
         <v>-1</v>
       </c>
       <c r="N34">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="O34" s="68"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -75208,16 +75191,16 @@
         <v>30</v>
       </c>
       <c r="M35">
-        <f t="shared" ref="M35:N35" si="28" xml:space="preserve"> E25 - E35</f>
+        <f t="shared" ref="M35:N35" si="32" xml:space="preserve"> E25 - E35</f>
         <v>0</v>
       </c>
       <c r="N35">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O35" s="68"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -75248,16 +75231,16 @@
         <v>40</v>
       </c>
       <c r="M36">
-        <f t="shared" ref="M36:N36" si="29" xml:space="preserve"> E26 - E36</f>
+        <f t="shared" ref="M36:N36" si="33" xml:space="preserve"> E26 - E36</f>
         <v>0</v>
       </c>
       <c r="N36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="O36" s="66"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -75288,16 +75271,16 @@
         <v>50</v>
       </c>
       <c r="M37">
-        <f t="shared" ref="M37:N37" si="30" xml:space="preserve"> E27 - E37</f>
+        <f t="shared" ref="M37:N37" si="34" xml:space="preserve"> E27 - E37</f>
         <v>0</v>
       </c>
       <c r="N37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="O37" s="68"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -75328,16 +75311,16 @@
         <v>60</v>
       </c>
       <c r="M38">
-        <f t="shared" ref="M38:N38" si="31" xml:space="preserve"> E28 - E38</f>
+        <f t="shared" ref="M38:N38" si="35" xml:space="preserve"> E28 - E38</f>
         <v>0</v>
       </c>
       <c r="N38">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="O38" s="68"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -75368,16 +75351,16 @@
         <v>70</v>
       </c>
       <c r="M39">
-        <f t="shared" ref="M39:N39" si="32" xml:space="preserve"> E29 - E39</f>
+        <f t="shared" ref="M39:N39" si="36" xml:space="preserve"> E29 - E39</f>
         <v>0</v>
       </c>
       <c r="N39">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O39" s="68"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -75408,16 +75391,16 @@
         <v>80</v>
       </c>
       <c r="M40">
-        <f t="shared" ref="M40:N40" si="33" xml:space="preserve"> E30 - E40</f>
+        <f t="shared" ref="M40:N40" si="37" xml:space="preserve"> E30 - E40</f>
         <v>1</v>
       </c>
       <c r="N40">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="O40" s="68"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -75457,7 +75440,7 @@
       </c>
       <c r="O41" s="68"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -75476,12 +75459,12 @@
       <c r="F42" s="65">
         <v>0</v>
       </c>
-      <c r="G42" s="77"/>
-      <c r="H42" s="77"/>
+      <c r="G42" s="72"/>
+      <c r="H42" s="72"/>
       <c r="N42" s="67"/>
       <c r="O42" s="68"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -75500,12 +75483,10 @@
       <c r="F43" s="65">
         <v>0</v>
       </c>
-      <c r="G43" s="77"/>
-      <c r="H43" s="77"/>
-      <c r="N43" s="67"/>
-      <c r="O43" s="68"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G43" s="72"/>
+      <c r="H43" s="72"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -75524,13 +75505,17 @@
       <c r="F44" s="65">
         <v>25</v>
       </c>
-      <c r="G44" s="77"/>
-      <c r="H44" s="77"/>
-      <c r="N44" s="73"/>
-      <c r="O44" s="74"/>
-      <c r="P44" s="74"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G44" s="72"/>
+      <c r="H44" s="72"/>
+      <c r="K44" t="s">
+        <v>146</v>
+      </c>
+      <c r="L44">
+        <f xml:space="preserve"> AVERAGE(M22:M41)</f>
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -75549,13 +75534,17 @@
       <c r="F45" s="65">
         <v>0</v>
       </c>
-      <c r="G45" s="77"/>
-      <c r="H45" s="77"/>
-      <c r="N45" s="75"/>
-      <c r="O45" s="65"/>
-      <c r="P45" s="65"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G45" s="72"/>
+      <c r="H45" s="72"/>
+      <c r="K45" t="s">
+        <v>147</v>
+      </c>
+      <c r="L45">
+        <f xml:space="preserve"> AVERAGE(M2:M21)</f>
+        <v>2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -75574,13 +75563,21 @@
       <c r="F46" s="65">
         <v>0</v>
       </c>
-      <c r="G46" s="77"/>
-      <c r="H46" s="77"/>
-      <c r="N46" s="75"/>
-      <c r="O46" s="65"/>
-      <c r="P46" s="65"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G46" s="72"/>
+      <c r="H46" s="72"/>
+      <c r="K46" t="s">
+        <v>148</v>
+      </c>
+      <c r="L46">
+        <f xml:space="preserve"> AVERAGE(S2:S21)</f>
+        <v>2.65</v>
+      </c>
+      <c r="N46">
+        <f xml:space="preserve"> 0.15*0.15</f>
+        <v>2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -75599,13 +75596,10 @@
       <c r="F47" s="65">
         <v>15</v>
       </c>
-      <c r="G47" s="77"/>
-      <c r="H47" s="77"/>
-      <c r="N47" s="75"/>
-      <c r="O47" s="65"/>
-      <c r="P47" s="65"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G47" s="72"/>
+      <c r="H47" s="72"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -75624,13 +75618,10 @@
       <c r="F48" s="65">
         <v>38</v>
       </c>
-      <c r="G48" s="77"/>
-      <c r="H48" s="77"/>
-      <c r="N48" s="75"/>
-      <c r="O48" s="65"/>
-      <c r="P48" s="65"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G48" s="72"/>
+      <c r="H48" s="72"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -75649,13 +75640,14 @@
       <c r="F49" s="65">
         <v>43</v>
       </c>
-      <c r="G49" s="77"/>
-      <c r="H49" s="77"/>
-      <c r="N49" s="75"/>
-      <c r="O49" s="65"/>
-      <c r="P49" s="65"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G49" s="72"/>
+      <c r="H49" s="72"/>
+      <c r="L49">
+        <f xml:space="preserve"> L44 / N46</f>
+        <v>-4.4444444444444446</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -75674,13 +75666,14 @@
       <c r="F50" s="65">
         <v>0</v>
       </c>
-      <c r="G50" s="77"/>
-      <c r="H50" s="77"/>
-      <c r="N50" s="75"/>
-      <c r="O50" s="65"/>
-      <c r="P50" s="65"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G50" s="72"/>
+      <c r="H50" s="72"/>
+      <c r="L50">
+        <f xml:space="preserve"> L45 / N46</f>
+        <v>113.33333333333333</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -75699,13 +75692,14 @@
       <c r="F51" s="65">
         <v>5</v>
       </c>
-      <c r="G51" s="77"/>
-      <c r="H51" s="77"/>
-      <c r="N51" s="75"/>
-      <c r="O51" s="65"/>
-      <c r="P51" s="65"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G51" s="72"/>
+      <c r="H51" s="72"/>
+      <c r="L51">
+        <f xml:space="preserve"> L46 / N46</f>
+        <v>117.77777777777777</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -75724,13 +75718,10 @@
       <c r="F52" s="65">
         <v>0</v>
       </c>
-      <c r="G52" s="77"/>
-      <c r="H52" s="77"/>
-      <c r="N52" s="75"/>
-      <c r="O52" s="65"/>
-      <c r="P52" s="65"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G52" s="72"/>
+      <c r="H52" s="72"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>9</v>
       </c>
@@ -75749,13 +75740,10 @@
       <c r="F53" s="65">
         <v>2</v>
       </c>
-      <c r="G53" s="77"/>
-      <c r="H53" s="77"/>
-      <c r="N53" s="75"/>
-      <c r="O53" s="65"/>
-      <c r="P53" s="65"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G53" s="72"/>
+      <c r="H53" s="72"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>9</v>
       </c>
@@ -75774,13 +75762,10 @@
       <c r="F54" s="65">
         <v>0</v>
       </c>
-      <c r="G54" s="77"/>
-      <c r="H54" s="77"/>
-      <c r="N54" s="75"/>
-      <c r="O54" s="65"/>
-      <c r="P54" s="65"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G54" s="72"/>
+      <c r="H54" s="72"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>9</v>
       </c>
@@ -75799,13 +75784,10 @@
       <c r="F55" s="65">
         <v>0</v>
       </c>
-      <c r="G55" s="77"/>
-      <c r="H55" s="77"/>
-      <c r="N55" s="73"/>
-      <c r="O55" s="74"/>
-      <c r="P55" s="74"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G55" s="72"/>
+      <c r="H55" s="72"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>9</v>
       </c>
@@ -75824,13 +75806,10 @@
       <c r="F56" s="65">
         <v>0</v>
       </c>
-      <c r="G56" s="77"/>
-      <c r="H56" s="77"/>
-      <c r="N56" s="75"/>
-      <c r="O56" s="65"/>
-      <c r="P56" s="65"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G56" s="72"/>
+      <c r="H56" s="72"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>9</v>
       </c>
@@ -75849,13 +75828,10 @@
       <c r="F57" s="65">
         <v>0</v>
       </c>
-      <c r="G57" s="77"/>
-      <c r="H57" s="77"/>
-      <c r="N57" s="75"/>
-      <c r="O57" s="65"/>
-      <c r="P57" s="65"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G57" s="72"/>
+      <c r="H57" s="72"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>9</v>
       </c>
@@ -75874,13 +75850,10 @@
       <c r="F58" s="65">
         <v>7</v>
       </c>
-      <c r="G58" s="77"/>
-      <c r="H58" s="77"/>
-      <c r="N58" s="75"/>
-      <c r="O58" s="65"/>
-      <c r="P58" s="65"/>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G58" s="72"/>
+      <c r="H58" s="72"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>9</v>
       </c>
@@ -75899,13 +75872,10 @@
       <c r="F59" s="65">
         <v>4</v>
       </c>
-      <c r="G59" s="77"/>
-      <c r="H59" s="77"/>
-      <c r="N59" s="75"/>
-      <c r="O59" s="65"/>
-      <c r="P59" s="65"/>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G59" s="72"/>
+      <c r="H59" s="72"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>9</v>
       </c>
@@ -75924,13 +75894,10 @@
       <c r="F60" s="65">
         <v>0</v>
       </c>
-      <c r="G60" s="77"/>
-      <c r="H60" s="77"/>
-      <c r="N60" s="75"/>
-      <c r="O60" s="65"/>
-      <c r="P60" s="65"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G60" s="72"/>
+      <c r="H60" s="72"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>9</v>
       </c>
@@ -75949,13 +75916,10 @@
       <c r="F61" s="65">
         <v>1</v>
       </c>
-      <c r="G61" s="77"/>
-      <c r="H61" s="77"/>
-      <c r="N61" s="75"/>
-      <c r="O61" s="65"/>
-      <c r="P61" s="65"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G61" s="72"/>
+      <c r="H61" s="72"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -75974,13 +75938,10 @@
       <c r="F62" s="65">
         <v>0</v>
       </c>
-      <c r="G62" s="77"/>
-      <c r="H62" s="77"/>
-      <c r="N62" s="75"/>
-      <c r="O62" s="65"/>
-      <c r="P62" s="65"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G62" s="72"/>
+      <c r="H62" s="72"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -75999,13 +75960,10 @@
       <c r="F63" s="65">
         <v>4</v>
       </c>
-      <c r="G63" s="77"/>
-      <c r="H63" s="77"/>
-      <c r="N63" s="75"/>
-      <c r="O63" s="65"/>
-      <c r="P63" s="65"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G63" s="72"/>
+      <c r="H63" s="72"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -76024,13 +75982,10 @@
       <c r="F64" s="65">
         <v>4</v>
       </c>
-      <c r="G64" s="77"/>
-      <c r="H64" s="77"/>
-      <c r="N64" s="75"/>
-      <c r="O64" s="65"/>
-      <c r="P64" s="65"/>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G64" s="72"/>
+      <c r="H64" s="72"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -76049,13 +76004,10 @@
       <c r="F65" s="65">
         <v>12</v>
       </c>
-      <c r="G65" s="77"/>
-      <c r="H65" s="77"/>
-      <c r="N65" s="75"/>
-      <c r="O65" s="65"/>
-      <c r="P65" s="65"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G65" s="72"/>
+      <c r="H65" s="72"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -76074,13 +76026,10 @@
       <c r="F66" s="65">
         <v>1</v>
       </c>
-      <c r="G66" s="77"/>
-      <c r="H66" s="77"/>
-      <c r="N66" s="71"/>
-      <c r="O66" s="72"/>
-      <c r="P66" s="72"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G66" s="72"/>
+      <c r="H66" s="72"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -76099,13 +76048,10 @@
       <c r="F67" s="65">
         <v>6</v>
       </c>
-      <c r="G67" s="77"/>
-      <c r="H67" s="77"/>
-      <c r="N67" s="73"/>
-      <c r="O67" s="74"/>
-      <c r="P67" s="74"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G67" s="72"/>
+      <c r="H67" s="72"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -76124,13 +76070,10 @@
       <c r="F68" s="65">
         <v>0</v>
       </c>
-      <c r="G68" s="77"/>
-      <c r="H68" s="77"/>
-      <c r="N68" s="75"/>
-      <c r="O68" s="65"/>
-      <c r="P68" s="65"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G68" s="72"/>
+      <c r="H68" s="72"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -76149,13 +76092,10 @@
       <c r="F69" s="65">
         <v>0</v>
       </c>
-      <c r="G69" s="77"/>
-      <c r="H69" s="77"/>
-      <c r="N69" s="75"/>
-      <c r="O69" s="65"/>
-      <c r="P69" s="65"/>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G69" s="72"/>
+      <c r="H69" s="72"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -76174,13 +76114,10 @@
       <c r="F70" s="65">
         <v>0</v>
       </c>
-      <c r="G70" s="77"/>
-      <c r="H70" s="77"/>
-      <c r="N70" s="75"/>
-      <c r="O70" s="65"/>
-      <c r="P70" s="65"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G70" s="72"/>
+      <c r="H70" s="72"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -76199,13 +76136,10 @@
       <c r="F71" s="65">
         <v>1</v>
       </c>
-      <c r="G71" s="77"/>
-      <c r="H71" s="77"/>
-      <c r="N71" s="75"/>
-      <c r="O71" s="65"/>
-      <c r="P71" s="65"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G71" s="72"/>
+      <c r="H71" s="72"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -76224,13 +76158,10 @@
       <c r="F72" s="65">
         <v>0</v>
       </c>
-      <c r="G72" s="77"/>
-      <c r="H72" s="77"/>
-      <c r="N72" s="75"/>
-      <c r="O72" s="65"/>
-      <c r="P72" s="65"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G72" s="72"/>
+      <c r="H72" s="72"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -76249,13 +76180,10 @@
       <c r="F73" s="65">
         <v>4</v>
       </c>
-      <c r="G73" s="77"/>
-      <c r="H73" s="77"/>
-      <c r="N73" s="75"/>
-      <c r="O73" s="65"/>
-      <c r="P73" s="65"/>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G73" s="72"/>
+      <c r="H73" s="72"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -76274,13 +76202,10 @@
       <c r="F74" s="65">
         <v>1</v>
       </c>
-      <c r="G74" s="77"/>
-      <c r="H74" s="77"/>
-      <c r="N74" s="75"/>
-      <c r="O74" s="65"/>
-      <c r="P74" s="65"/>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G74" s="72"/>
+      <c r="H74" s="72"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -76299,13 +76224,10 @@
       <c r="F75" s="65">
         <v>0</v>
       </c>
-      <c r="G75" s="77"/>
-      <c r="H75" s="77"/>
-      <c r="N75" s="75"/>
-      <c r="O75" s="65"/>
-      <c r="P75" s="65"/>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G75" s="72"/>
+      <c r="H75" s="72"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -76324,13 +76246,10 @@
       <c r="F76" s="65">
         <v>3</v>
       </c>
-      <c r="G76" s="77"/>
-      <c r="H76" s="77"/>
-      <c r="N76" s="75"/>
-      <c r="O76" s="65"/>
-      <c r="P76" s="65"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G76" s="72"/>
+      <c r="H76" s="72"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -76349,13 +76268,10 @@
       <c r="F77" s="65">
         <v>0</v>
       </c>
-      <c r="G77" s="77"/>
-      <c r="H77" s="77"/>
-      <c r="N77" s="75"/>
-      <c r="O77" s="65"/>
-      <c r="P77" s="65"/>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G77" s="72"/>
+      <c r="H77" s="72"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>14</v>
       </c>
@@ -76374,13 +76290,10 @@
       <c r="F78" s="65">
         <v>0</v>
       </c>
-      <c r="G78" s="77"/>
-      <c r="H78" s="77"/>
-      <c r="N78" s="73"/>
-      <c r="O78" s="74"/>
-      <c r="P78" s="74"/>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G78" s="72"/>
+      <c r="H78" s="72"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>14</v>
       </c>
@@ -76399,13 +76312,10 @@
       <c r="F79" s="65">
         <v>0</v>
       </c>
-      <c r="G79" s="77"/>
-      <c r="H79" s="77"/>
-      <c r="N79" s="75"/>
-      <c r="O79" s="65"/>
-      <c r="P79" s="65"/>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G79" s="72"/>
+      <c r="H79" s="72"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -76424,13 +76334,10 @@
       <c r="F80" s="65">
         <v>0</v>
       </c>
-      <c r="G80" s="77"/>
-      <c r="H80" s="77"/>
-      <c r="N80" s="75"/>
-      <c r="O80" s="65"/>
-      <c r="P80" s="65"/>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G80" s="72"/>
+      <c r="H80" s="72"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -76449,74 +76356,134 @@
       <c r="F81" s="65">
         <v>1</v>
       </c>
-      <c r="G81" s="77"/>
-      <c r="H81" s="77"/>
-      <c r="N81" s="75"/>
-      <c r="O81" s="65"/>
-      <c r="P81" s="65"/>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="E82" s="76"/>
-      <c r="F82" s="76"/>
-      <c r="G82" s="76"/>
-      <c r="H82" s="76"/>
-      <c r="N82" s="75"/>
-      <c r="O82" s="65"/>
-      <c r="P82" s="65"/>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="E83" s="76"/>
-      <c r="F83" s="76"/>
-      <c r="G83" s="76"/>
-      <c r="H83" s="76"/>
-      <c r="N83" s="75"/>
-      <c r="O83" s="65"/>
-      <c r="P83" s="65"/>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="E84" s="76"/>
-      <c r="F84" s="76"/>
-      <c r="G84" s="76"/>
-      <c r="H84" s="76"/>
-      <c r="N84" s="75"/>
-      <c r="O84" s="65"/>
-      <c r="P84" s="65"/>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="E85" s="76"/>
-      <c r="F85" s="76"/>
-      <c r="G85" s="76"/>
-      <c r="H85" s="76"/>
-      <c r="N85" s="75"/>
-      <c r="O85" s="65"/>
-      <c r="P85" s="65"/>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="E86" s="76"/>
-      <c r="F86" s="76"/>
-      <c r="G86" s="76"/>
-      <c r="H86" s="76"/>
-      <c r="N86" s="75"/>
-      <c r="O86" s="65"/>
-      <c r="P86" s="65"/>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="E87" s="76"/>
-      <c r="F87" s="76"/>
-      <c r="G87" s="76"/>
-      <c r="H87" s="76"/>
-      <c r="N87" s="75"/>
-      <c r="O87" s="65"/>
-      <c r="P87" s="65"/>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="E88" s="76"/>
-      <c r="F88" s="76"/>
-      <c r="G88" s="76"/>
-      <c r="H88" s="76"/>
-      <c r="N88" s="75"/>
-      <c r="O88" s="65"/>
-      <c r="P88" s="65"/>
+      <c r="G81" s="72"/>
+      <c r="H81" s="72"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E82" s="71"/>
+      <c r="F82" s="71"/>
+      <c r="G82" s="71"/>
+      <c r="H82" s="71"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E83" s="71"/>
+      <c r="F83" s="71"/>
+      <c r="G83" s="71"/>
+      <c r="H83" s="71"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E84" s="71"/>
+      <c r="F84" s="71"/>
+      <c r="G84" s="71"/>
+      <c r="H84" s="71"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C85" t="s">
+        <v>152</v>
+      </c>
+      <c r="D85" t="s">
+        <v>149</v>
+      </c>
+      <c r="E85" s="71">
+        <f xml:space="preserve"> AVERAGE(E2:E41)</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F85" s="71">
+        <f xml:space="preserve"> E85 /N46</f>
+        <v>24.444444444444446</v>
+      </c>
+      <c r="G85" s="71"/>
+      <c r="H85" s="71"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
+        <v>152</v>
+      </c>
+      <c r="D86" t="s">
+        <v>151</v>
+      </c>
+      <c r="E86" s="71">
+        <f xml:space="preserve"> AVERAGE(E2:E11,E22:E31)</f>
+        <v>0.5</v>
+      </c>
+      <c r="F86" s="71"/>
+      <c r="G86" s="71"/>
+      <c r="H86" s="71"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C87" t="s">
+        <v>152</v>
+      </c>
+      <c r="D87" t="s">
+        <v>150</v>
+      </c>
+      <c r="E87" s="71">
+        <f xml:space="preserve"> AVERAGE(E12:E21,E32:E41)</f>
+        <v>0.6</v>
+      </c>
+      <c r="F87" s="71"/>
+      <c r="G87" s="71"/>
+      <c r="H87" s="71"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E88" s="71"/>
+      <c r="F88" s="71"/>
+      <c r="G88" s="71"/>
+      <c r="H88" s="71"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C89" t="s">
+        <v>153</v>
+      </c>
+      <c r="D89" t="s">
+        <v>149</v>
+      </c>
+      <c r="E89">
+        <f xml:space="preserve"> AVERAGE(E42:E81)</f>
+        <v>3.875</v>
+      </c>
+      <c r="F89" s="71">
+        <f xml:space="preserve"> E89 /N46</f>
+        <v>172.22222222222223</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D90" t="s">
+        <v>151</v>
+      </c>
+      <c r="E90">
+        <f xml:space="preserve"> AVERAGE(E42:E51,E62:E71)</f>
+        <v>5.15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D91" t="s">
+        <v>150</v>
+      </c>
+      <c r="E91">
+        <f xml:space="preserve"> AVERAGE(E52:E61,E72:E81)</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E94">
+        <f xml:space="preserve"> 5.15 - 0.55</f>
+        <v>4.6000000000000005</v>
+      </c>
+      <c r="F94">
+        <f xml:space="preserve"> E94/N46</f>
+        <v>204.44444444444449</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E95">
+        <f xml:space="preserve"> 2.6-0.6</f>
+        <v>2</v>
+      </c>
+      <c r="F95">
+        <f xml:space="preserve"> E95/N46</f>
+        <v>88.888888888888886</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Thesis coming along, working on disc
</commit_message>
<xml_diff>
--- a/Analysis/Data/2018 Tiles Allison's Computer.xlsx
+++ b/Analysis/Data/2018 Tiles Allison's Computer.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Tiles" sheetId="2" r:id="rId1"/>
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6401" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6490" uniqueCount="160">
   <si>
     <t>Stream</t>
   </si>
@@ -733,6 +733,24 @@
   </si>
   <si>
     <t>Post</t>
+  </si>
+  <si>
+    <t>BACI Density</t>
+  </si>
+  <si>
+    <t>Y Density</t>
+  </si>
+  <si>
+    <t>N Density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stream </t>
+  </si>
+  <si>
+    <t>2017 density</t>
+  </si>
+  <si>
+    <t>2018 density</t>
   </si>
 </sst>
 </file>
@@ -73504,15 +73522,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T95"/>
+  <dimension ref="A1:AA95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="I96" sqref="I96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -73559,8 +73577,20 @@
       <c r="T1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W1" t="s">
+        <v>157</v>
+      </c>
+      <c r="X1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -73568,7 +73598,7 @@
         <v>2017</v>
       </c>
       <c r="C2" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D2" s="67">
         <v>0</v>
@@ -73591,11 +73621,11 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2:M11" si="0" xml:space="preserve"> E42 - E52</f>
+        <f xml:space="preserve"> E42 - E52</f>
         <v>2</v>
       </c>
       <c r="N2">
-        <f t="shared" ref="N2:N11" si="1" xml:space="preserve"> F42 - F52</f>
+        <f xml:space="preserve"> F42 - F52</f>
         <v>0</v>
       </c>
       <c r="O2" s="66"/>
@@ -73613,8 +73643,22 @@
         <f xml:space="preserve"> N2- N22</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W2" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X2" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y2" s="67">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="68">
+        <f xml:space="preserve"> E42 - E2</f>
+        <v>5</v>
+      </c>
+      <c r="AA2" s="68"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -73622,7 +73666,7 @@
         <v>2017</v>
       </c>
       <c r="C3" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D3" s="67">
         <v>10</v>
@@ -73645,11 +73689,11 @@
         <v>10</v>
       </c>
       <c r="M3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> E43 - E53</f>
         <v>-3</v>
       </c>
       <c r="N3">
-        <f t="shared" si="1"/>
+        <f xml:space="preserve"> F43 - F53</f>
         <v>-2</v>
       </c>
       <c r="O3" s="68"/>
@@ -73660,15 +73704,29 @@
         <v>10</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:T3" si="2" xml:space="preserve"> M3- M23</f>
+        <f t="shared" ref="S3:T3" si="0" xml:space="preserve"> M3- M23</f>
         <v>-5</v>
       </c>
       <c r="T3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W3" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X3" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y3" s="67">
+        <v>10</v>
+      </c>
+      <c r="Z3" s="68">
+        <f xml:space="preserve"> E43 - E3</f>
+        <v>-1</v>
+      </c>
+      <c r="AA3" s="68"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -73676,7 +73734,7 @@
         <v>2017</v>
       </c>
       <c r="C4" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D4" s="67">
         <v>20</v>
@@ -73699,11 +73757,11 @@
         <v>20</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> E44 - E54</f>
         <v>17</v>
       </c>
       <c r="N4">
-        <f t="shared" si="1"/>
+        <f xml:space="preserve"> F44 - F54</f>
         <v>25</v>
       </c>
       <c r="O4" s="68"/>
@@ -73714,15 +73772,29 @@
         <v>20</v>
       </c>
       <c r="S4">
-        <f t="shared" ref="S4:T4" si="3" xml:space="preserve"> M4- M24</f>
+        <f t="shared" ref="S4:T4" si="1" xml:space="preserve"> M4- M24</f>
         <v>15</v>
       </c>
       <c r="T4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W4" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X4" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y4" s="67">
+        <v>20</v>
+      </c>
+      <c r="Z4" s="68">
+        <f xml:space="preserve"> E44 - E4</f>
+        <v>15</v>
+      </c>
+      <c r="AA4" s="68"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -73730,7 +73802,7 @@
         <v>2017</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D5" s="67">
         <v>30</v>
@@ -73753,11 +73825,11 @@
         <v>30</v>
       </c>
       <c r="M5">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> E45 - E55</f>
         <v>2</v>
       </c>
       <c r="N5">
-        <f t="shared" si="1"/>
+        <f xml:space="preserve"> F45 - F55</f>
         <v>0</v>
       </c>
       <c r="O5" s="68"/>
@@ -73768,15 +73840,29 @@
         <v>30</v>
       </c>
       <c r="S5">
-        <f t="shared" ref="S5:T5" si="4" xml:space="preserve"> M5- M25</f>
+        <f t="shared" ref="S5:T5" si="2" xml:space="preserve"> M5- M25</f>
         <v>2</v>
       </c>
       <c r="T5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W5" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X5" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y5" s="67">
+        <v>30</v>
+      </c>
+      <c r="Z5" s="68">
+        <f xml:space="preserve"> E45 - E5</f>
+        <v>3</v>
+      </c>
+      <c r="AA5" s="68"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -73784,7 +73870,7 @@
         <v>2017</v>
       </c>
       <c r="C6" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D6" s="67">
         <v>40</v>
@@ -73807,11 +73893,11 @@
         <v>40</v>
       </c>
       <c r="M6">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> E46 - E56</f>
         <v>3</v>
       </c>
       <c r="N6">
-        <f t="shared" si="1"/>
+        <f xml:space="preserve"> F46 - F56</f>
         <v>0</v>
       </c>
       <c r="O6" s="68"/>
@@ -73822,15 +73908,29 @@
         <v>40</v>
       </c>
       <c r="S6">
-        <f t="shared" ref="S6:T6" si="5" xml:space="preserve"> M6- M26</f>
+        <f t="shared" ref="S6:T6" si="3" xml:space="preserve"> M6- M26</f>
         <v>1</v>
       </c>
       <c r="T6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="W6" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X6" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y6" s="67">
+        <v>40</v>
+      </c>
+      <c r="Z6" s="68">
+        <f xml:space="preserve"> E46 - E6</f>
+        <v>2</v>
+      </c>
+      <c r="AA6" s="68"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -73838,7 +73938,7 @@
         <v>2017</v>
       </c>
       <c r="C7" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D7" s="67">
         <v>50</v>
@@ -73861,11 +73961,11 @@
         <v>50</v>
       </c>
       <c r="M7">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> E47 - E57</f>
         <v>-1</v>
       </c>
       <c r="N7">
-        <f t="shared" si="1"/>
+        <f xml:space="preserve"> F47 - F57</f>
         <v>15</v>
       </c>
       <c r="O7" s="68"/>
@@ -73876,15 +73976,29 @@
         <v>50</v>
       </c>
       <c r="S7">
-        <f t="shared" ref="S7:T7" si="6" xml:space="preserve"> M7- M27</f>
+        <f t="shared" ref="S7:T7" si="4" xml:space="preserve"> M7- M27</f>
         <v>0</v>
       </c>
       <c r="T7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W7" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X7" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y7" s="67">
+        <v>50</v>
+      </c>
+      <c r="Z7" s="68">
+        <f xml:space="preserve"> E47 - E7</f>
+        <v>-1</v>
+      </c>
+      <c r="AA7" s="68"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -73892,7 +74006,7 @@
         <v>2017</v>
       </c>
       <c r="C8" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D8" s="67">
         <v>60</v>
@@ -73915,11 +74029,11 @@
         <v>60</v>
       </c>
       <c r="M8">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> E48 - E58</f>
         <v>1</v>
       </c>
       <c r="N8">
-        <f t="shared" si="1"/>
+        <f xml:space="preserve"> F48 - F58</f>
         <v>31</v>
       </c>
       <c r="O8" s="68"/>
@@ -73930,15 +74044,29 @@
         <v>60</v>
       </c>
       <c r="S8">
-        <f t="shared" ref="S8:T8" si="7" xml:space="preserve"> M8- M28</f>
+        <f t="shared" ref="S8:T8" si="5" xml:space="preserve"> M8- M28</f>
         <v>2</v>
       </c>
       <c r="T8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W8" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X8" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y8" s="67">
+        <v>60</v>
+      </c>
+      <c r="Z8" s="68">
+        <f xml:space="preserve"> E48 - E8</f>
+        <v>1</v>
+      </c>
+      <c r="AA8" s="68"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -73946,7 +74074,7 @@
         <v>2017</v>
       </c>
       <c r="C9" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D9" s="67">
         <v>70</v>
@@ -73969,11 +74097,11 @@
         <v>70</v>
       </c>
       <c r="M9">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> E49 - E59</f>
         <v>-1</v>
       </c>
       <c r="N9">
-        <f t="shared" si="1"/>
+        <f xml:space="preserve"> F49 - F59</f>
         <v>39</v>
       </c>
       <c r="O9" s="68"/>
@@ -73984,15 +74112,29 @@
         <v>70</v>
       </c>
       <c r="S9">
-        <f t="shared" ref="S9:T9" si="8" xml:space="preserve"> M9- M29</f>
+        <f t="shared" ref="S9:T9" si="6" xml:space="preserve"> M9- M29</f>
         <v>1</v>
       </c>
       <c r="T9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W9" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X9" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y9" s="67">
+        <v>70</v>
+      </c>
+      <c r="Z9" s="68">
+        <f xml:space="preserve"> E49 - E9</f>
+        <v>1</v>
+      </c>
+      <c r="AA9" s="68"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -74000,7 +74142,7 @@
         <v>2017</v>
       </c>
       <c r="C10" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D10" s="67">
         <v>80</v>
@@ -74023,11 +74165,11 @@
         <v>80</v>
       </c>
       <c r="M10">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> E50 - E60</f>
         <v>1</v>
       </c>
       <c r="N10">
-        <f t="shared" si="1"/>
+        <f xml:space="preserve"> F50 - F60</f>
         <v>0</v>
       </c>
       <c r="O10" s="68"/>
@@ -74038,15 +74180,29 @@
         <v>80</v>
       </c>
       <c r="S10">
-        <f t="shared" ref="S10:T10" si="9" xml:space="preserve"> M10- M30</f>
+        <f t="shared" ref="S10:T10" si="7" xml:space="preserve"> M10- M30</f>
         <v>3</v>
       </c>
       <c r="T10">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W10" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X10" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y10" s="67">
+        <v>80</v>
+      </c>
+      <c r="Z10" s="68">
+        <f xml:space="preserve"> E50 - E10</f>
+        <v>1</v>
+      </c>
+      <c r="AA10" s="68"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -74054,7 +74210,7 @@
         <v>2017</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D11" s="67">
         <v>90</v>
@@ -74077,11 +74233,11 @@
         <v>90</v>
       </c>
       <c r="M11">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> E51 - E61</f>
         <v>2</v>
       </c>
       <c r="N11">
-        <f t="shared" si="1"/>
+        <f xml:space="preserve"> F51 - F61</f>
         <v>4</v>
       </c>
       <c r="O11" s="68"/>
@@ -74092,15 +74248,29 @@
         <v>90</v>
       </c>
       <c r="S11">
-        <f t="shared" ref="S11:T11" si="10" xml:space="preserve"> M11- M31</f>
+        <f t="shared" ref="S11:T11" si="8" xml:space="preserve"> M11- M31</f>
         <v>3</v>
       </c>
       <c r="T11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W11" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X11" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y11" s="67">
+        <v>90</v>
+      </c>
+      <c r="Z11" s="68">
+        <f xml:space="preserve"> E51 - E11</f>
+        <v>2</v>
+      </c>
+      <c r="AA11" s="68"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -74108,7 +74278,7 @@
         <v>2017</v>
       </c>
       <c r="C12" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D12" s="67">
         <v>0</v>
@@ -74131,11 +74301,11 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" ref="M12:M21" si="11" xml:space="preserve"> E62 - E72</f>
+        <f xml:space="preserve"> E62 - E72</f>
         <v>9</v>
       </c>
       <c r="N12">
-        <f t="shared" ref="N12:N21" si="12" xml:space="preserve"> F62 - F72</f>
+        <f xml:space="preserve"> F62 - F72</f>
         <v>0</v>
       </c>
       <c r="O12" s="68"/>
@@ -74153,8 +74323,22 @@
         <f xml:space="preserve"> N12 - N32</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W12" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X12" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y12" s="67">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="68">
+        <f xml:space="preserve"> E52 - E12</f>
+        <v>0</v>
+      </c>
+      <c r="AA12" s="68"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -74162,7 +74346,7 @@
         <v>2017</v>
       </c>
       <c r="C13" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D13" s="67">
         <v>10</v>
@@ -74185,11 +74369,11 @@
         <v>10</v>
       </c>
       <c r="M13">
-        <f t="shared" si="11"/>
+        <f xml:space="preserve"> E63 - E73</f>
         <v>16</v>
       </c>
       <c r="N13">
-        <f t="shared" si="12"/>
+        <f xml:space="preserve"> F63 - F73</f>
         <v>0</v>
       </c>
       <c r="O13" s="66"/>
@@ -74200,15 +74384,29 @@
         <v>10</v>
       </c>
       <c r="S13">
-        <f t="shared" ref="S13:T13" si="13" xml:space="preserve"> M13 - M33</f>
+        <f t="shared" ref="S13:T13" si="9" xml:space="preserve"> M13 - M33</f>
         <v>14</v>
       </c>
       <c r="T13">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="W13" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X13" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y13" s="67">
+        <v>10</v>
+      </c>
+      <c r="Z13" s="68">
+        <f xml:space="preserve"> E53 - E13</f>
+        <v>4</v>
+      </c>
+      <c r="AA13" s="68"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -74216,7 +74414,7 @@
         <v>2017</v>
       </c>
       <c r="C14" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D14" s="67">
         <v>20</v>
@@ -74239,11 +74437,11 @@
         <v>20</v>
       </c>
       <c r="M14">
-        <f t="shared" si="11"/>
+        <f xml:space="preserve"> E64 - E74</f>
         <v>12</v>
       </c>
       <c r="N14">
-        <f t="shared" si="12"/>
+        <f xml:space="preserve"> F64 - F74</f>
         <v>3</v>
       </c>
       <c r="O14" s="68"/>
@@ -74254,15 +74452,29 @@
         <v>20</v>
       </c>
       <c r="S14">
-        <f t="shared" ref="S14:T14" si="14" xml:space="preserve"> M14 - M34</f>
+        <f t="shared" ref="S14:T14" si="10" xml:space="preserve"> M14 - M34</f>
         <v>13</v>
       </c>
       <c r="T14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W14" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X14" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y14" s="67">
+        <v>20</v>
+      </c>
+      <c r="Z14" s="68">
+        <f xml:space="preserve"> E54 - E14</f>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="68"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -74270,7 +74482,7 @@
         <v>2017</v>
       </c>
       <c r="C15" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D15" s="67">
         <v>30</v>
@@ -74293,11 +74505,11 @@
         <v>30</v>
       </c>
       <c r="M15">
-        <f t="shared" si="11"/>
+        <f xml:space="preserve"> E65 - E75</f>
         <v>4</v>
       </c>
       <c r="N15">
-        <f t="shared" si="12"/>
+        <f xml:space="preserve"> F65 - F75</f>
         <v>12</v>
       </c>
       <c r="O15" s="68"/>
@@ -74308,15 +74520,29 @@
         <v>30</v>
       </c>
       <c r="S15">
-        <f t="shared" ref="S15:T15" si="15" xml:space="preserve"> M15 - M35</f>
+        <f t="shared" ref="S15:T15" si="11" xml:space="preserve"> M15 - M35</f>
         <v>4</v>
       </c>
       <c r="T15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W15" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X15" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y15" s="67">
+        <v>30</v>
+      </c>
+      <c r="Z15" s="68">
+        <f xml:space="preserve"> E55 - E15</f>
+        <v>1</v>
+      </c>
+      <c r="AA15" s="68"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -74324,7 +74550,7 @@
         <v>2017</v>
       </c>
       <c r="C16" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D16" s="67">
         <v>40</v>
@@ -74347,11 +74573,11 @@
         <v>40</v>
       </c>
       <c r="M16">
-        <f t="shared" si="11"/>
+        <f xml:space="preserve"> E66 - E76</f>
         <v>-3</v>
       </c>
       <c r="N16">
-        <f t="shared" si="12"/>
+        <f xml:space="preserve"> F66 - F76</f>
         <v>-2</v>
       </c>
       <c r="O16" s="68"/>
@@ -74362,15 +74588,29 @@
         <v>40</v>
       </c>
       <c r="S16">
-        <f t="shared" ref="S16:T16" si="16" xml:space="preserve"> M16 - M36</f>
+        <f t="shared" ref="S16:T16" si="12" xml:space="preserve"> M16 - M36</f>
         <v>-3</v>
       </c>
       <c r="T16">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W16" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X16" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y16" s="67">
+        <v>40</v>
+      </c>
+      <c r="Z16" s="68">
+        <f xml:space="preserve"> E56 - E16</f>
+        <v>1</v>
+      </c>
+      <c r="AA16" s="68"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -74378,7 +74618,7 @@
         <v>2017</v>
       </c>
       <c r="C17" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D17" s="67">
         <v>50</v>
@@ -74401,11 +74641,11 @@
         <v>50</v>
       </c>
       <c r="M17">
-        <f t="shared" si="11"/>
+        <f xml:space="preserve"> E67 - E77</f>
         <v>-2</v>
       </c>
       <c r="N17">
-        <f t="shared" si="12"/>
+        <f xml:space="preserve"> F67 - F77</f>
         <v>6</v>
       </c>
       <c r="O17" s="68"/>
@@ -74416,15 +74656,29 @@
         <v>50</v>
       </c>
       <c r="S17">
-        <f t="shared" ref="S17:T17" si="17" xml:space="preserve"> M17 - M37</f>
+        <f t="shared" ref="S17:T17" si="13" xml:space="preserve"> M17 - M37</f>
         <v>-2</v>
       </c>
       <c r="T17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W17" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X17" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y17" s="67">
+        <v>50</v>
+      </c>
+      <c r="Z17" s="68">
+        <f xml:space="preserve"> E57 - E17</f>
+        <v>-1</v>
+      </c>
+      <c r="AA17" s="68"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -74432,7 +74686,7 @@
         <v>2017</v>
       </c>
       <c r="C18" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D18" s="67">
         <v>60</v>
@@ -74455,11 +74709,11 @@
         <v>60</v>
       </c>
       <c r="M18">
-        <f t="shared" si="11"/>
+        <f xml:space="preserve"> E68 - E78</f>
         <v>4</v>
       </c>
       <c r="N18">
-        <f t="shared" si="12"/>
+        <f xml:space="preserve"> F68 - F78</f>
         <v>0</v>
       </c>
       <c r="O18" s="68"/>
@@ -74470,15 +74724,29 @@
         <v>60</v>
       </c>
       <c r="S18">
-        <f t="shared" ref="S18:T18" si="18" xml:space="preserve"> M18 - M38</f>
+        <f t="shared" ref="S18:T18" si="14" xml:space="preserve"> M18 - M38</f>
         <v>4</v>
       </c>
       <c r="T18">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="W18" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X18" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y18" s="67">
+        <v>60</v>
+      </c>
+      <c r="Z18" s="68">
+        <f xml:space="preserve"> E58 - E18</f>
+        <v>-1</v>
+      </c>
+      <c r="AA18" s="68"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -74486,7 +74754,7 @@
         <v>2017</v>
       </c>
       <c r="C19" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D19" s="67">
         <v>70</v>
@@ -74509,11 +74777,11 @@
         <v>70</v>
       </c>
       <c r="M19">
-        <f t="shared" si="11"/>
+        <f xml:space="preserve"> E69 - E79</f>
         <v>0</v>
       </c>
       <c r="N19">
-        <f t="shared" si="12"/>
+        <f xml:space="preserve"> F69 - F79</f>
         <v>0</v>
       </c>
       <c r="O19" s="68"/>
@@ -74524,15 +74792,29 @@
         <v>70</v>
       </c>
       <c r="S19">
-        <f t="shared" ref="S19:T19" si="19" xml:space="preserve"> M19 - M39</f>
+        <f t="shared" ref="S19:T19" si="15" xml:space="preserve"> M19 - M39</f>
         <v>0</v>
       </c>
       <c r="T19">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="W19" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X19" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y19" s="67">
+        <v>70</v>
+      </c>
+      <c r="Z19" s="68">
+        <f xml:space="preserve"> E59 - E19</f>
+        <v>0</v>
+      </c>
+      <c r="AA19" s="68"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -74540,7 +74822,7 @@
         <v>2017</v>
       </c>
       <c r="C20" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D20" s="67">
         <v>80</v>
@@ -74563,11 +74845,11 @@
         <v>80</v>
       </c>
       <c r="M20">
-        <f t="shared" si="11"/>
+        <f xml:space="preserve"> E70 - E80</f>
         <v>-6</v>
       </c>
       <c r="N20">
-        <f t="shared" si="12"/>
+        <f xml:space="preserve"> F70 - F80</f>
         <v>0</v>
       </c>
       <c r="O20" s="68"/>
@@ -74578,15 +74860,29 @@
         <v>80</v>
       </c>
       <c r="S20">
-        <f t="shared" ref="S20:T20" si="20" xml:space="preserve"> M20 - M40</f>
+        <f t="shared" ref="S20:T20" si="16" xml:space="preserve"> M20 - M40</f>
         <v>-7</v>
       </c>
       <c r="T20">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="W20" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X20" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y20" s="67">
+        <v>80</v>
+      </c>
+      <c r="Z20" s="68">
+        <f xml:space="preserve"> E60 - E20</f>
+        <v>-2</v>
+      </c>
+      <c r="AA20" s="68"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -74594,7 +74890,7 @@
         <v>2017</v>
       </c>
       <c r="C21" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D21" s="67">
         <v>90</v>
@@ -74617,11 +74913,11 @@
         <v>90</v>
       </c>
       <c r="M21">
-        <f t="shared" si="11"/>
+        <f xml:space="preserve"> E71 - E81</f>
         <v>-6</v>
       </c>
       <c r="N21">
-        <f t="shared" si="12"/>
+        <f xml:space="preserve"> F71 - F81</f>
         <v>0</v>
       </c>
       <c r="O21" s="68"/>
@@ -74632,15 +74928,29 @@
         <v>90</v>
       </c>
       <c r="S21">
-        <f t="shared" ref="S21:T21" si="21" xml:space="preserve"> M21 - M41</f>
+        <f t="shared" ref="S21:T21" si="17" xml:space="preserve"> M21 - M41</f>
         <v>-6</v>
       </c>
       <c r="T21">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="W21" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="X21" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y21" s="67">
+        <v>90</v>
+      </c>
+      <c r="Z21" s="68">
+        <f xml:space="preserve"> E61 - E21</f>
+        <v>-1</v>
+      </c>
+      <c r="AA21" s="68"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -74648,7 +74958,7 @@
         <v>2017</v>
       </c>
       <c r="C22" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D22" s="67">
         <v>0</v>
@@ -74679,8 +74989,22 @@
         <v>0</v>
       </c>
       <c r="O22" s="68"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W22" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X22" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y22" s="67">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="68">
+        <f xml:space="preserve"> E62 - E22</f>
+        <v>13</v>
+      </c>
+      <c r="AA22" s="68"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -74688,7 +75012,7 @@
         <v>2017</v>
       </c>
       <c r="C23" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D23" s="67">
         <v>10</v>
@@ -74719,8 +75043,22 @@
         <v>0</v>
       </c>
       <c r="O23" s="68"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W23" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X23" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y23" s="67">
+        <v>10</v>
+      </c>
+      <c r="Z23" s="68">
+        <f xml:space="preserve"> E63 - E23</f>
+        <v>14</v>
+      </c>
+      <c r="AA23" s="68"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -74728,7 +75066,7 @@
         <v>2017</v>
       </c>
       <c r="C24" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D24" s="67">
         <v>20</v>
@@ -74751,16 +75089,30 @@
         <v>20</v>
       </c>
       <c r="M24">
-        <f t="shared" ref="M24:N24" si="22" xml:space="preserve"> E4 - E14</f>
+        <f t="shared" ref="M24:N24" si="18" xml:space="preserve"> E4 - E14</f>
         <v>2</v>
       </c>
       <c r="N24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O24" s="69"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W24" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X24" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y24" s="67">
+        <v>20</v>
+      </c>
+      <c r="Z24" s="68">
+        <f xml:space="preserve"> E64 - E24</f>
+        <v>12</v>
+      </c>
+      <c r="AA24" s="68"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -74768,7 +75120,7 @@
         <v>2017</v>
       </c>
       <c r="C25" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D25" s="67">
         <v>30</v>
@@ -74791,16 +75143,30 @@
         <v>30</v>
       </c>
       <c r="M25">
-        <f t="shared" ref="M25:N25" si="23" xml:space="preserve"> E5 - E15</f>
+        <f t="shared" ref="M25:N25" si="19" xml:space="preserve"> E5 - E15</f>
         <v>0</v>
       </c>
       <c r="N25">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O25" s="66"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W25" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X25" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y25" s="67">
+        <v>30</v>
+      </c>
+      <c r="Z25" s="68">
+        <f xml:space="preserve"> E65 - E25</f>
+        <v>9</v>
+      </c>
+      <c r="AA25" s="68"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -74808,7 +75174,7 @@
         <v>2017</v>
       </c>
       <c r="C26" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D26" s="67">
         <v>40</v>
@@ -74831,16 +75197,30 @@
         <v>40</v>
       </c>
       <c r="M26">
-        <f t="shared" ref="M26:N26" si="24" xml:space="preserve"> E6 - E16</f>
+        <f t="shared" ref="M26:N26" si="20" xml:space="preserve"> E6 - E16</f>
         <v>2</v>
       </c>
       <c r="N26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O26" s="68"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W26" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X26" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y26" s="67">
+        <v>40</v>
+      </c>
+      <c r="Z26" s="68">
+        <f xml:space="preserve"> E66 - E26</f>
+        <v>1</v>
+      </c>
+      <c r="AA26" s="68"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -74848,7 +75228,7 @@
         <v>2017</v>
       </c>
       <c r="C27" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D27" s="67">
         <v>50</v>
@@ -74871,16 +75251,30 @@
         <v>50</v>
       </c>
       <c r="M27">
-        <f t="shared" ref="M27:N27" si="25" xml:space="preserve"> E7 - E17</f>
+        <f t="shared" ref="M27:N27" si="21" xml:space="preserve"> E7 - E17</f>
         <v>-1</v>
       </c>
       <c r="N27">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="O27" s="68"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W27" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X27" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y27" s="67">
+        <v>50</v>
+      </c>
+      <c r="Z27" s="68">
+        <f xml:space="preserve"> E67 - E27</f>
+        <v>5</v>
+      </c>
+      <c r="AA27" s="68"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -74888,7 +75282,7 @@
         <v>2017</v>
       </c>
       <c r="C28" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D28" s="67">
         <v>60</v>
@@ -74911,16 +75305,30 @@
         <v>60</v>
       </c>
       <c r="M28">
-        <f t="shared" ref="M28:N28" si="26" xml:space="preserve"> E8 - E18</f>
+        <f t="shared" ref="M28:N28" si="22" xml:space="preserve"> E8 - E18</f>
         <v>-1</v>
       </c>
       <c r="N28">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="O28" s="68"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W28" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X28" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y28" s="67">
+        <v>60</v>
+      </c>
+      <c r="Z28" s="68">
+        <f xml:space="preserve"> E68 - E28</f>
+        <v>4</v>
+      </c>
+      <c r="AA28" s="68"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -74928,7 +75336,7 @@
         <v>2017</v>
       </c>
       <c r="C29" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D29" s="67">
         <v>70</v>
@@ -74951,16 +75359,30 @@
         <v>70</v>
       </c>
       <c r="M29">
-        <f t="shared" ref="M29:N29" si="27" xml:space="preserve"> E9 - E19</f>
+        <f t="shared" ref="M29:N29" si="23" xml:space="preserve"> E9 - E19</f>
         <v>-2</v>
       </c>
       <c r="N29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="O29" s="68"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W29" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X29" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y29" s="67">
+        <v>70</v>
+      </c>
+      <c r="Z29" s="68">
+        <f xml:space="preserve"> E69 - E29</f>
+        <v>1</v>
+      </c>
+      <c r="AA29" s="68"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -74968,7 +75390,7 @@
         <v>2017</v>
       </c>
       <c r="C30" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D30" s="67">
         <v>80</v>
@@ -74991,16 +75413,30 @@
         <v>80</v>
       </c>
       <c r="M30">
-        <f t="shared" ref="M30:N30" si="28" xml:space="preserve"> E10 - E20</f>
+        <f t="shared" ref="M30:N30" si="24" xml:space="preserve"> E10 - E20</f>
         <v>-2</v>
       </c>
       <c r="N30">
-        <f t="shared" si="28"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="O30" s="68"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W30" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X30" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y30" s="67">
+        <v>80</v>
+      </c>
+      <c r="Z30" s="68">
+        <f xml:space="preserve"> E70 - E30</f>
+        <v>3</v>
+      </c>
+      <c r="AA30" s="68"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -75008,7 +75444,7 @@
         <v>2017</v>
       </c>
       <c r="C31" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D31" s="67">
         <v>90</v>
@@ -75031,16 +75467,30 @@
         <v>90</v>
       </c>
       <c r="M31">
-        <f t="shared" ref="M31:N31" si="29" xml:space="preserve"> E11 - E21</f>
+        <f t="shared" ref="M31:N31" si="25" xml:space="preserve"> E11 - E21</f>
         <v>-1</v>
       </c>
       <c r="N31">
-        <f t="shared" si="29"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="O31" s="68"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="W31" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X31" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y31" s="67">
+        <v>90</v>
+      </c>
+      <c r="Z31" s="68">
+        <f xml:space="preserve"> E71 - E31</f>
+        <v>3</v>
+      </c>
+      <c r="AA31" s="68"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -75048,7 +75498,7 @@
         <v>2017</v>
       </c>
       <c r="C32" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D32" s="67">
         <v>0</v>
@@ -75079,8 +75529,22 @@
         <v>0</v>
       </c>
       <c r="O32" s="68"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="W32" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X32" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y32" s="67">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="68">
+        <f xml:space="preserve"> E72 - E32</f>
+        <v>4</v>
+      </c>
+      <c r="AA32" s="68"/>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -75088,7 +75552,7 @@
         <v>2017</v>
       </c>
       <c r="C33" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D33" s="67">
         <v>10</v>
@@ -75111,16 +75575,30 @@
         <v>10</v>
       </c>
       <c r="M33">
-        <f t="shared" ref="M33:N33" si="30" xml:space="preserve"> E23 - E33</f>
+        <f t="shared" ref="M33:N33" si="26" xml:space="preserve"> E23 - E33</f>
         <v>2</v>
       </c>
       <c r="N33">
-        <f t="shared" si="30"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O33" s="68"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="W33" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X33" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y33" s="67">
+        <v>10</v>
+      </c>
+      <c r="Z33" s="68">
+        <f xml:space="preserve"> E73 - E33</f>
+        <v>0</v>
+      </c>
+      <c r="AA33" s="68"/>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -75128,7 +75606,7 @@
         <v>2017</v>
       </c>
       <c r="C34" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D34" s="67">
         <v>20</v>
@@ -75151,16 +75629,30 @@
         <v>20</v>
       </c>
       <c r="M34">
-        <f t="shared" ref="M34:N34" si="31" xml:space="preserve"> E24 - E34</f>
+        <f t="shared" ref="M34:N34" si="27" xml:space="preserve"> E24 - E34</f>
         <v>-1</v>
       </c>
       <c r="N34">
-        <f t="shared" si="31"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="O34" s="68"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="W34" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X34" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y34" s="67">
+        <v>20</v>
+      </c>
+      <c r="Z34" s="68">
+        <f xml:space="preserve"> E74 - E34</f>
+        <v>-1</v>
+      </c>
+      <c r="AA34" s="68"/>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -75168,7 +75660,7 @@
         <v>2017</v>
       </c>
       <c r="C35" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D35" s="67">
         <v>30</v>
@@ -75191,16 +75683,30 @@
         <v>30</v>
       </c>
       <c r="M35">
-        <f t="shared" ref="M35:N35" si="32" xml:space="preserve"> E25 - E35</f>
+        <f t="shared" ref="M35:N35" si="28" xml:space="preserve"> E25 - E35</f>
         <v>0</v>
       </c>
       <c r="N35">
-        <f t="shared" si="32"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="O35" s="68"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="W35" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X35" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y35" s="67">
+        <v>30</v>
+      </c>
+      <c r="Z35" s="68">
+        <f xml:space="preserve"> E75 - E35</f>
+        <v>5</v>
+      </c>
+      <c r="AA35" s="68"/>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -75208,7 +75714,7 @@
         <v>2017</v>
       </c>
       <c r="C36" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D36" s="67">
         <v>40</v>
@@ -75231,16 +75737,30 @@
         <v>40</v>
       </c>
       <c r="M36">
-        <f t="shared" ref="M36:N36" si="33" xml:space="preserve"> E26 - E36</f>
+        <f t="shared" ref="M36:N36" si="29" xml:space="preserve"> E26 - E36</f>
         <v>0</v>
       </c>
       <c r="N36">
-        <f t="shared" si="33"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="O36" s="66"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="W36" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X36" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y36" s="67">
+        <v>40</v>
+      </c>
+      <c r="Z36" s="68">
+        <f xml:space="preserve"> E76 - E36</f>
+        <v>4</v>
+      </c>
+      <c r="AA36" s="68"/>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -75248,7 +75768,7 @@
         <v>2017</v>
       </c>
       <c r="C37" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D37" s="67">
         <v>50</v>
@@ -75271,16 +75791,30 @@
         <v>50</v>
       </c>
       <c r="M37">
-        <f t="shared" ref="M37:N37" si="34" xml:space="preserve"> E27 - E37</f>
+        <f t="shared" ref="M37:N37" si="30" xml:space="preserve"> E27 - E37</f>
         <v>0</v>
       </c>
       <c r="N37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="O37" s="68"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="W37" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X37" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y37" s="67">
+        <v>50</v>
+      </c>
+      <c r="Z37" s="68">
+        <f xml:space="preserve"> E77 - E37</f>
+        <v>7</v>
+      </c>
+      <c r="AA37" s="68"/>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -75288,7 +75822,7 @@
         <v>2017</v>
       </c>
       <c r="C38" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D38" s="67">
         <v>60</v>
@@ -75311,16 +75845,30 @@
         <v>60</v>
       </c>
       <c r="M38">
-        <f t="shared" ref="M38:N38" si="35" xml:space="preserve"> E28 - E38</f>
+        <f t="shared" ref="M38:N38" si="31" xml:space="preserve"> E28 - E38</f>
         <v>0</v>
       </c>
       <c r="N38">
-        <f t="shared" si="35"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="O38" s="68"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="W38" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X38" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y38" s="67">
+        <v>60</v>
+      </c>
+      <c r="Z38" s="68">
+        <f xml:space="preserve"> E78 - E38</f>
+        <v>0</v>
+      </c>
+      <c r="AA38" s="68"/>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -75328,7 +75876,7 @@
         <v>2017</v>
       </c>
       <c r="C39" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D39" s="67">
         <v>70</v>
@@ -75351,16 +75899,30 @@
         <v>70</v>
       </c>
       <c r="M39">
-        <f t="shared" ref="M39:N39" si="36" xml:space="preserve"> E29 - E39</f>
+        <f t="shared" ref="M39:N39" si="32" xml:space="preserve"> E29 - E39</f>
         <v>0</v>
       </c>
       <c r="N39">
-        <f t="shared" si="36"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O39" s="68"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="W39" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X39" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y39" s="67">
+        <v>70</v>
+      </c>
+      <c r="Z39" s="68">
+        <f xml:space="preserve"> E79 - E39</f>
+        <v>1</v>
+      </c>
+      <c r="AA39" s="68"/>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -75368,7 +75930,7 @@
         <v>2017</v>
       </c>
       <c r="C40" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D40" s="67">
         <v>80</v>
@@ -75391,16 +75953,30 @@
         <v>80</v>
       </c>
       <c r="M40">
-        <f t="shared" ref="M40:N40" si="37" xml:space="preserve"> E30 - E40</f>
+        <f t="shared" ref="M40:N40" si="33" xml:space="preserve"> E30 - E40</f>
         <v>1</v>
       </c>
       <c r="N40">
-        <f t="shared" si="37"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="O40" s="68"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="W40" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X40" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y40" s="67">
+        <v>80</v>
+      </c>
+      <c r="Z40" s="68">
+        <f xml:space="preserve"> E80 - E40</f>
+        <v>10</v>
+      </c>
+      <c r="AA40" s="68"/>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -75408,7 +75984,7 @@
         <v>2017</v>
       </c>
       <c r="C41" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D41" s="67">
         <v>90</v>
@@ -75439,8 +76015,22 @@
         <v>0</v>
       </c>
       <c r="O41" s="68"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="W41" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="X41" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y41" s="67">
+        <v>90</v>
+      </c>
+      <c r="Z41" s="68">
+        <f xml:space="preserve"> E81 - E41</f>
+        <v>9</v>
+      </c>
+      <c r="AA41" s="68"/>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -75448,7 +76038,7 @@
         <v>2018</v>
       </c>
       <c r="C42" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D42" s="67">
         <v>0</v>
@@ -75463,8 +76053,12 @@
       <c r="H42" s="72"/>
       <c r="N42" s="67"/>
       <c r="O42" s="68"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="W42" s="72"/>
+      <c r="X42" s="72"/>
+      <c r="Z42" s="72"/>
+      <c r="AA42" s="72"/>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -75472,7 +76066,7 @@
         <v>2018</v>
       </c>
       <c r="C43" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D43" s="67">
         <v>10</v>
@@ -75485,8 +76079,12 @@
       </c>
       <c r="G43" s="72"/>
       <c r="H43" s="72"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="W43" s="72"/>
+      <c r="X43" s="72"/>
+      <c r="Z43" s="72"/>
+      <c r="AA43" s="72"/>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -75494,7 +76092,7 @@
         <v>2018</v>
       </c>
       <c r="C44" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D44" s="67">
         <v>20</v>
@@ -75514,8 +76112,12 @@
         <f xml:space="preserve"> AVERAGE(M22:M41)</f>
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="W44" s="72"/>
+      <c r="X44" s="72"/>
+      <c r="Z44" s="72"/>
+      <c r="AA44" s="72"/>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -75523,7 +76125,7 @@
         <v>2018</v>
       </c>
       <c r="C45" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D45" s="67">
         <v>30</v>
@@ -75543,8 +76145,12 @@
         <f xml:space="preserve"> AVERAGE(M2:M21)</f>
         <v>2.5499999999999998</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="W45" s="72"/>
+      <c r="X45" s="72"/>
+      <c r="Z45" s="72"/>
+      <c r="AA45" s="72"/>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -75552,7 +76158,7 @@
         <v>2018</v>
       </c>
       <c r="C46" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D46" s="67">
         <v>40</v>
@@ -75576,8 +76182,12 @@
         <f xml:space="preserve"> 0.15*0.15</f>
         <v>2.2499999999999999E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="W46" s="72"/>
+      <c r="X46" s="72"/>
+      <c r="Z46" s="72"/>
+      <c r="AA46" s="72"/>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -75585,7 +76195,7 @@
         <v>2018</v>
       </c>
       <c r="C47" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D47" s="67">
         <v>50</v>
@@ -75598,8 +76208,12 @@
       </c>
       <c r="G47" s="72"/>
       <c r="H47" s="72"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="W47" s="72"/>
+      <c r="X47" s="72"/>
+      <c r="Z47" s="72"/>
+      <c r="AA47" s="72"/>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -75607,7 +76221,7 @@
         <v>2018</v>
       </c>
       <c r="C48" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D48" s="67">
         <v>60</v>
@@ -75620,8 +76234,12 @@
       </c>
       <c r="G48" s="72"/>
       <c r="H48" s="72"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="W48" s="72"/>
+      <c r="X48" s="72"/>
+      <c r="Z48" s="72"/>
+      <c r="AA48" s="72"/>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -75629,7 +76247,7 @@
         <v>2018</v>
       </c>
       <c r="C49" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D49" s="67">
         <v>70</v>
@@ -75642,12 +76260,19 @@
       </c>
       <c r="G49" s="72"/>
       <c r="H49" s="72"/>
+      <c r="K49" t="s">
+        <v>158</v>
+      </c>
       <c r="L49">
         <f xml:space="preserve"> L44 / N46</f>
         <v>-4.4444444444444446</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="W49" s="72"/>
+      <c r="X49" s="72"/>
+      <c r="Z49" s="72"/>
+      <c r="AA49" s="72"/>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -75655,7 +76280,7 @@
         <v>2018</v>
       </c>
       <c r="C50" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D50" s="67">
         <v>80</v>
@@ -75668,12 +76293,19 @@
       </c>
       <c r="G50" s="72"/>
       <c r="H50" s="72"/>
+      <c r="K50" t="s">
+        <v>159</v>
+      </c>
       <c r="L50">
         <f xml:space="preserve"> L45 / N46</f>
         <v>113.33333333333333</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="W50" s="72"/>
+      <c r="X50" s="72"/>
+      <c r="Z50" s="72"/>
+      <c r="AA50" s="72"/>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -75681,7 +76313,7 @@
         <v>2018</v>
       </c>
       <c r="C51" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D51" s="67">
         <v>90</v>
@@ -75694,12 +76326,19 @@
       </c>
       <c r="G51" s="72"/>
       <c r="H51" s="72"/>
+      <c r="K51" t="s">
+        <v>154</v>
+      </c>
       <c r="L51">
         <f xml:space="preserve"> L46 / N46</f>
         <v>117.77777777777777</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="W51" s="72"/>
+      <c r="X51" s="72"/>
+      <c r="Z51" s="72"/>
+      <c r="AA51" s="72"/>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -75707,7 +76346,7 @@
         <v>2018</v>
       </c>
       <c r="C52" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D52" s="67">
         <v>0</v>
@@ -75720,8 +76359,12 @@
       </c>
       <c r="G52" s="72"/>
       <c r="H52" s="72"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="W52" s="72"/>
+      <c r="X52" s="72"/>
+      <c r="Z52" s="72"/>
+      <c r="AA52" s="72"/>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>9</v>
       </c>
@@ -75729,7 +76372,7 @@
         <v>2018</v>
       </c>
       <c r="C53" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D53" s="67">
         <v>10</v>
@@ -75742,8 +76385,12 @@
       </c>
       <c r="G53" s="72"/>
       <c r="H53" s="72"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="W53" s="72"/>
+      <c r="X53" s="72"/>
+      <c r="Z53" s="72"/>
+      <c r="AA53" s="72"/>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>9</v>
       </c>
@@ -75751,7 +76398,7 @@
         <v>2018</v>
       </c>
       <c r="C54" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D54" s="67">
         <v>20</v>
@@ -75764,8 +76411,12 @@
       </c>
       <c r="G54" s="72"/>
       <c r="H54" s="72"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="W54" s="72"/>
+      <c r="X54" s="72"/>
+      <c r="Z54" s="72"/>
+      <c r="AA54" s="72"/>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>9</v>
       </c>
@@ -75773,7 +76424,7 @@
         <v>2018</v>
       </c>
       <c r="C55" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D55" s="67">
         <v>30</v>
@@ -75786,8 +76437,12 @@
       </c>
       <c r="G55" s="72"/>
       <c r="H55" s="72"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="W55" s="72"/>
+      <c r="X55" s="72"/>
+      <c r="Z55" s="72"/>
+      <c r="AA55" s="72"/>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>9</v>
       </c>
@@ -75795,7 +76450,7 @@
         <v>2018</v>
       </c>
       <c r="C56" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D56" s="67">
         <v>40</v>
@@ -75808,8 +76463,12 @@
       </c>
       <c r="G56" s="72"/>
       <c r="H56" s="72"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="W56" s="72"/>
+      <c r="X56" s="72"/>
+      <c r="Z56" s="72"/>
+      <c r="AA56" s="72"/>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>9</v>
       </c>
@@ -75817,7 +76476,7 @@
         <v>2018</v>
       </c>
       <c r="C57" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D57" s="67">
         <v>50</v>
@@ -75830,8 +76489,12 @@
       </c>
       <c r="G57" s="72"/>
       <c r="H57" s="72"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="W57" s="72"/>
+      <c r="X57" s="72"/>
+      <c r="Z57" s="72"/>
+      <c r="AA57" s="72"/>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>9</v>
       </c>
@@ -75839,7 +76502,7 @@
         <v>2018</v>
       </c>
       <c r="C58" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D58" s="67">
         <v>60</v>
@@ -75852,8 +76515,12 @@
       </c>
       <c r="G58" s="72"/>
       <c r="H58" s="72"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="W58" s="72"/>
+      <c r="X58" s="72"/>
+      <c r="Z58" s="72"/>
+      <c r="AA58" s="72"/>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>9</v>
       </c>
@@ -75861,7 +76528,7 @@
         <v>2018</v>
       </c>
       <c r="C59" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D59" s="67">
         <v>70</v>
@@ -75874,8 +76541,12 @@
       </c>
       <c r="G59" s="72"/>
       <c r="H59" s="72"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="W59" s="72"/>
+      <c r="X59" s="72"/>
+      <c r="Z59" s="72"/>
+      <c r="AA59" s="72"/>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>9</v>
       </c>
@@ -75883,7 +76554,7 @@
         <v>2018</v>
       </c>
       <c r="C60" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D60" s="67">
         <v>80</v>
@@ -75896,8 +76567,12 @@
       </c>
       <c r="G60" s="72"/>
       <c r="H60" s="72"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="W60" s="72"/>
+      <c r="X60" s="72"/>
+      <c r="Z60" s="72"/>
+      <c r="AA60" s="72"/>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>9</v>
       </c>
@@ -75905,7 +76580,7 @@
         <v>2018</v>
       </c>
       <c r="C61" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D61" s="67">
         <v>90</v>
@@ -75918,8 +76593,12 @@
       </c>
       <c r="G61" s="72"/>
       <c r="H61" s="72"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="W61" s="72"/>
+      <c r="X61" s="72"/>
+      <c r="Z61" s="72"/>
+      <c r="AA61" s="72"/>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -75927,7 +76606,7 @@
         <v>2018</v>
       </c>
       <c r="C62" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D62" s="67">
         <v>0</v>
@@ -75940,8 +76619,12 @@
       </c>
       <c r="G62" s="72"/>
       <c r="H62" s="72"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="W62" s="72"/>
+      <c r="X62" s="72"/>
+      <c r="Z62" s="72"/>
+      <c r="AA62" s="72"/>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -75949,7 +76632,7 @@
         <v>2018</v>
       </c>
       <c r="C63" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D63" s="67">
         <v>10</v>
@@ -75962,8 +76645,12 @@
       </c>
       <c r="G63" s="72"/>
       <c r="H63" s="72"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="W63" s="72"/>
+      <c r="X63" s="72"/>
+      <c r="Z63" s="72"/>
+      <c r="AA63" s="72"/>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -75971,7 +76658,7 @@
         <v>2018</v>
       </c>
       <c r="C64" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D64" s="67">
         <v>20</v>
@@ -75984,8 +76671,12 @@
       </c>
       <c r="G64" s="72"/>
       <c r="H64" s="72"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W64" s="72"/>
+      <c r="X64" s="72"/>
+      <c r="Z64" s="72"/>
+      <c r="AA64" s="72"/>
+    </row>
+    <row r="65" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -75993,7 +76684,7 @@
         <v>2018</v>
       </c>
       <c r="C65" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D65" s="67">
         <v>30</v>
@@ -76006,8 +76697,12 @@
       </c>
       <c r="G65" s="72"/>
       <c r="H65" s="72"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W65" s="72"/>
+      <c r="X65" s="72"/>
+      <c r="Z65" s="72"/>
+      <c r="AA65" s="72"/>
+    </row>
+    <row r="66" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -76015,7 +76710,7 @@
         <v>2018</v>
       </c>
       <c r="C66" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D66" s="67">
         <v>40</v>
@@ -76028,8 +76723,12 @@
       </c>
       <c r="G66" s="72"/>
       <c r="H66" s="72"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W66" s="72"/>
+      <c r="X66" s="72"/>
+      <c r="Z66" s="72"/>
+      <c r="AA66" s="72"/>
+    </row>
+    <row r="67" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -76037,7 +76736,7 @@
         <v>2018</v>
       </c>
       <c r="C67" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D67" s="67">
         <v>50</v>
@@ -76050,8 +76749,12 @@
       </c>
       <c r="G67" s="72"/>
       <c r="H67" s="72"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W67" s="72"/>
+      <c r="X67" s="72"/>
+      <c r="Z67" s="72"/>
+      <c r="AA67" s="72"/>
+    </row>
+    <row r="68" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -76059,7 +76762,7 @@
         <v>2018</v>
       </c>
       <c r="C68" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D68" s="67">
         <v>60</v>
@@ -76072,8 +76775,12 @@
       </c>
       <c r="G68" s="72"/>
       <c r="H68" s="72"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W68" s="72"/>
+      <c r="X68" s="72"/>
+      <c r="Z68" s="72"/>
+      <c r="AA68" s="72"/>
+    </row>
+    <row r="69" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -76081,7 +76788,7 @@
         <v>2018</v>
       </c>
       <c r="C69" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D69" s="67">
         <v>70</v>
@@ -76094,8 +76801,12 @@
       </c>
       <c r="G69" s="72"/>
       <c r="H69" s="72"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W69" s="72"/>
+      <c r="X69" s="72"/>
+      <c r="Z69" s="72"/>
+      <c r="AA69" s="72"/>
+    </row>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -76103,7 +76814,7 @@
         <v>2018</v>
       </c>
       <c r="C70" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D70" s="67">
         <v>80</v>
@@ -76116,8 +76827,12 @@
       </c>
       <c r="G70" s="72"/>
       <c r="H70" s="72"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W70" s="72"/>
+      <c r="X70" s="72"/>
+      <c r="Z70" s="72"/>
+      <c r="AA70" s="72"/>
+    </row>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -76125,7 +76840,7 @@
         <v>2018</v>
       </c>
       <c r="C71" s="70" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D71" s="67">
         <v>90</v>
@@ -76138,8 +76853,12 @@
       </c>
       <c r="G71" s="72"/>
       <c r="H71" s="72"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W71" s="72"/>
+      <c r="X71" s="72"/>
+      <c r="Z71" s="72"/>
+      <c r="AA71" s="72"/>
+    </row>
+    <row r="72" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -76147,7 +76866,7 @@
         <v>2018</v>
       </c>
       <c r="C72" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D72" s="67">
         <v>0</v>
@@ -76160,8 +76879,12 @@
       </c>
       <c r="G72" s="72"/>
       <c r="H72" s="72"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W72" s="72"/>
+      <c r="X72" s="72"/>
+      <c r="Z72" s="72"/>
+      <c r="AA72" s="72"/>
+    </row>
+    <row r="73" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -76169,7 +76892,7 @@
         <v>2018</v>
       </c>
       <c r="C73" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D73" s="67">
         <v>10</v>
@@ -76182,8 +76905,12 @@
       </c>
       <c r="G73" s="72"/>
       <c r="H73" s="72"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W73" s="72"/>
+      <c r="X73" s="72"/>
+      <c r="Z73" s="72"/>
+      <c r="AA73" s="72"/>
+    </row>
+    <row r="74" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -76191,7 +76918,7 @@
         <v>2018</v>
       </c>
       <c r="C74" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D74" s="67">
         <v>20</v>
@@ -76204,8 +76931,12 @@
       </c>
       <c r="G74" s="72"/>
       <c r="H74" s="72"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W74" s="72"/>
+      <c r="X74" s="72"/>
+      <c r="Z74" s="72"/>
+      <c r="AA74" s="72"/>
+    </row>
+    <row r="75" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -76213,7 +76944,7 @@
         <v>2018</v>
       </c>
       <c r="C75" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D75" s="67">
         <v>30</v>
@@ -76226,8 +76957,12 @@
       </c>
       <c r="G75" s="72"/>
       <c r="H75" s="72"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W75" s="72"/>
+      <c r="X75" s="72"/>
+      <c r="Z75" s="72"/>
+      <c r="AA75" s="72"/>
+    </row>
+    <row r="76" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -76235,7 +76970,7 @@
         <v>2018</v>
       </c>
       <c r="C76" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D76" s="67">
         <v>40</v>
@@ -76248,8 +76983,12 @@
       </c>
       <c r="G76" s="72"/>
       <c r="H76" s="72"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W76" s="72"/>
+      <c r="X76" s="72"/>
+      <c r="Z76" s="72"/>
+      <c r="AA76" s="72"/>
+    </row>
+    <row r="77" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -76257,7 +76996,7 @@
         <v>2018</v>
       </c>
       <c r="C77" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D77" s="67">
         <v>50</v>
@@ -76270,8 +77009,12 @@
       </c>
       <c r="G77" s="72"/>
       <c r="H77" s="72"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W77" s="72"/>
+      <c r="X77" s="72"/>
+      <c r="Z77" s="72"/>
+      <c r="AA77" s="72"/>
+    </row>
+    <row r="78" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>14</v>
       </c>
@@ -76279,7 +77022,7 @@
         <v>2018</v>
       </c>
       <c r="C78" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D78" s="67">
         <v>60</v>
@@ -76292,8 +77035,12 @@
       </c>
       <c r="G78" s="72"/>
       <c r="H78" s="72"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W78" s="72"/>
+      <c r="X78" s="72"/>
+      <c r="Z78" s="72"/>
+      <c r="AA78" s="72"/>
+    </row>
+    <row r="79" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>14</v>
       </c>
@@ -76301,7 +77048,7 @@
         <v>2018</v>
       </c>
       <c r="C79" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D79" s="67">
         <v>70</v>
@@ -76314,8 +77061,12 @@
       </c>
       <c r="G79" s="72"/>
       <c r="H79" s="72"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W79" s="72"/>
+      <c r="X79" s="72"/>
+      <c r="Z79" s="72"/>
+      <c r="AA79" s="72"/>
+    </row>
+    <row r="80" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -76323,7 +77074,7 @@
         <v>2018</v>
       </c>
       <c r="C80" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D80" s="67">
         <v>80</v>
@@ -76336,8 +77087,12 @@
       </c>
       <c r="G80" s="72"/>
       <c r="H80" s="72"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W80" s="72"/>
+      <c r="X80" s="72"/>
+      <c r="Z80" s="72"/>
+      <c r="AA80" s="72"/>
+    </row>
+    <row r="81" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -76345,7 +77100,7 @@
         <v>2018</v>
       </c>
       <c r="C81" s="70" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="D81" s="67">
         <v>90</v>
@@ -76358,26 +77113,42 @@
       </c>
       <c r="G81" s="72"/>
       <c r="H81" s="72"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W81" s="72"/>
+      <c r="X81" s="72"/>
+      <c r="Z81" s="72"/>
+      <c r="AA81" s="72"/>
+    </row>
+    <row r="82" spans="1:27" x14ac:dyDescent="0.2">
       <c r="E82" s="71"/>
       <c r="F82" s="71"/>
       <c r="G82" s="71"/>
       <c r="H82" s="71"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W82" s="71"/>
+      <c r="X82" s="71"/>
+      <c r="Z82" s="71"/>
+      <c r="AA82" s="71"/>
+    </row>
+    <row r="83" spans="1:27" x14ac:dyDescent="0.2">
       <c r="E83" s="71"/>
       <c r="F83" s="71"/>
       <c r="G83" s="71"/>
       <c r="H83" s="71"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W83" s="71"/>
+      <c r="X83" s="71"/>
+      <c r="Z83" s="71"/>
+      <c r="AA83" s="71"/>
+    </row>
+    <row r="84" spans="1:27" x14ac:dyDescent="0.2">
       <c r="E84" s="71"/>
       <c r="F84" s="71"/>
       <c r="G84" s="71"/>
       <c r="H84" s="71"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W84" s="71"/>
+      <c r="X84" s="71"/>
+      <c r="Z84" s="71"/>
+      <c r="AA84" s="71"/>
+    </row>
+    <row r="85" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C85" t="s">
         <v>152</v>
       </c>
@@ -76394,8 +77165,12 @@
       </c>
       <c r="G85" s="71"/>
       <c r="H85" s="71"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W85" s="71"/>
+      <c r="X85" s="71"/>
+      <c r="Z85" s="71"/>
+      <c r="AA85" s="71"/>
+    </row>
+    <row r="86" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C86" t="s">
         <v>152</v>
       </c>
@@ -76409,8 +77184,12 @@
       <c r="F86" s="71"/>
       <c r="G86" s="71"/>
       <c r="H86" s="71"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W86" s="71"/>
+      <c r="X86" s="71"/>
+      <c r="Z86" s="71"/>
+      <c r="AA86" s="71"/>
+    </row>
+    <row r="87" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C87" t="s">
         <v>152</v>
       </c>
@@ -76424,14 +77203,22 @@
       <c r="F87" s="71"/>
       <c r="G87" s="71"/>
       <c r="H87" s="71"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W87" s="71"/>
+      <c r="X87" s="71"/>
+      <c r="Z87" s="71"/>
+      <c r="AA87" s="71"/>
+    </row>
+    <row r="88" spans="1:27" x14ac:dyDescent="0.2">
       <c r="E88" s="71"/>
       <c r="F88" s="71"/>
       <c r="G88" s="71"/>
       <c r="H88" s="71"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="W88" s="71"/>
+      <c r="X88" s="71"/>
+      <c r="Z88" s="71"/>
+      <c r="AA88" s="71"/>
+    </row>
+    <row r="89" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C89" t="s">
         <v>153</v>
       </c>
@@ -76447,7 +77234,7 @@
         <v>172.22222222222223</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.2">
       <c r="D90" t="s">
         <v>151</v>
       </c>
@@ -76456,7 +77243,7 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.2">
       <c r="D91" t="s">
         <v>150</v>
       </c>
@@ -76465,7 +77252,10 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
+        <v>155</v>
+      </c>
       <c r="E94">
         <f xml:space="preserve"> 5.15 - 0.55</f>
         <v>4.6000000000000005</v>
@@ -76475,7 +77265,10 @@
         <v>204.44444444444449</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="D95" t="s">
+        <v>156</v>
+      </c>
       <c r="E95">
         <f xml:space="preserve"> 2.6-0.6</f>
         <v>2</v>

</xml_diff>